<commit_message>
not working click to chat in Firefox
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>number</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Yeshwanth</t>
+  </si>
+  <si>
+    <t>Testing {#name#}</t>
+  </si>
+  <si>
+    <t>__BLANK__</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +427,20 @@
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8800669077</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>